<commit_message>
import fields type added
</commit_message>
<xml_diff>
--- a/import_fld/field_import.xlsx
+++ b/import_fld/field_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\doxy\dist\import_fld\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Serge\PycharmProjects\docxy\import_fld\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>value_3</t>
   </si>
@@ -35,9 +35,6 @@
     <t>value_1</t>
   </si>
   <si>
-    <t>value_2</t>
-  </si>
-  <si>
     <t>test_field1</t>
   </si>
   <si>
@@ -50,100 +47,13 @@
     <t>test_field4</t>
   </si>
   <si>
-    <t>test_field5</t>
-  </si>
-  <si>
-    <t>test_field6</t>
-  </si>
-  <si>
-    <t>test_field7</t>
-  </si>
-  <si>
-    <t>test_field8</t>
-  </si>
-  <si>
-    <t>test_field9</t>
-  </si>
-  <si>
-    <t>test_field10</t>
-  </si>
-  <si>
-    <t>test_field11</t>
-  </si>
-  <si>
-    <t>test_field12</t>
-  </si>
-  <si>
-    <t>test_field13</t>
-  </si>
-  <si>
-    <t>test_field14</t>
-  </si>
-  <si>
-    <t>test_field15</t>
-  </si>
-  <si>
-    <t>test_field16</t>
-  </si>
-  <si>
-    <t>test_field17</t>
-  </si>
-  <si>
-    <t>test_field18</t>
-  </si>
-  <si>
-    <t>test_field19</t>
-  </si>
-  <si>
-    <t>test_field20</t>
-  </si>
-  <si>
-    <t>value_5</t>
-  </si>
-  <si>
-    <t>value_6</t>
-  </si>
-  <si>
-    <t>value_7</t>
-  </si>
-  <si>
-    <t>value_8</t>
-  </si>
-  <si>
-    <t>value_9</t>
-  </si>
-  <si>
-    <t>value_10</t>
-  </si>
-  <si>
-    <t>value_11</t>
-  </si>
-  <si>
-    <t>value_12</t>
-  </si>
-  <si>
-    <t>value_13</t>
-  </si>
-  <si>
-    <t>value_14</t>
-  </si>
-  <si>
-    <t>value_15</t>
-  </si>
-  <si>
-    <t>value_16</t>
-  </si>
-  <si>
-    <t>value_17</t>
-  </si>
-  <si>
-    <t>value_18</t>
-  </si>
-  <si>
-    <t>value_19</t>
-  </si>
-  <si>
-    <t>value_20</t>
+    <t>текст</t>
+  </si>
+  <si>
+    <t>дата</t>
+  </si>
+  <si>
+    <t>числа</t>
   </si>
 </sst>
 </file>
@@ -180,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -462,176 +373,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>34030</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
combi digits added to all_tags merge
</commit_message>
<xml_diff>
--- a/import_fld/field_import.xlsx
+++ b/import_fld/field_import.xlsx
@@ -24,36 +24,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>value_3</t>
-  </si>
-  <si>
-    <t>value_4</t>
-  </si>
-  <si>
-    <t>value_1</t>
-  </si>
-  <si>
-    <t>test_field1</t>
-  </si>
-  <si>
-    <t>test_field2</t>
-  </si>
-  <si>
-    <t>test_field3</t>
-  </si>
-  <si>
-    <t>test_field4</t>
-  </si>
-  <si>
-    <t>текст</t>
-  </si>
-  <si>
-    <t>дата</t>
-  </si>
-  <si>
-    <t>числа</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>full name</t>
+  </si>
+  <si>
+    <t>Elon Musk</t>
+  </si>
+  <si>
+    <t>adress</t>
+  </si>
+  <si>
+    <t>3500 Deer Creek Rd, Palo Alto, CA 94304, USA</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>info@tesla.com</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>JPMorgan Chase</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Palo Alto</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Tim Cook</t>
+  </si>
+  <si>
+    <t>1 Apple Park Way, Cupertino, CA 95014, USA</t>
+  </si>
+  <si>
+    <t>contact@apple.com</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>Cupertino</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Sundar Pichai</t>
+  </si>
+  <si>
+    <t>1600 Amphitheatre Parkway, Mountain View, CA 94043, USA</t>
+  </si>
+  <si>
+    <t>support@google.com</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Mountain View</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Satya Nadella</t>
+  </si>
+  <si>
+    <t>1 Microsoft Way, Redmond, WA 98052, USA</t>
+  </si>
+  <si>
+    <t>info@microsoft.com</t>
+  </si>
+  <si>
+    <t>Citibank</t>
+  </si>
+  <si>
+    <t>Redmond</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Jeff Bezos</t>
+  </si>
+  <si>
+    <t>410 Terry Ave N, Seattle, WA 98109, USA</t>
+  </si>
+  <si>
+    <t>support@amazon.com</t>
+  </si>
+  <si>
+    <t>Chase Bank</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Mark Zuckerberg</t>
+  </si>
+  <si>
+    <t>1 Hacker Way, Menlo Park, CA 94025, USA</t>
+  </si>
+  <si>
+    <t>info@facebook.com</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>Menlo Park</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Reed Hastings</t>
+  </si>
+  <si>
+    <t>100 Winchester Circle, Los Gatos, CA 95032, USA</t>
+  </si>
+  <si>
+    <t>contact@netflix.com</t>
+  </si>
+  <si>
+    <t>Goldman Sachs</t>
+  </si>
+  <si>
+    <t>Los Gatos</t>
   </si>
 </sst>
 </file>
@@ -90,9 +207,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -373,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,43 +503,359 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>34030</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>